<commit_message>
Modified Solution Listing Demo Sheet
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVMDemo-solution-listing.xlsx
+++ b/docs/OVW Sheets/OVMDemo-solution-listing.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arachapa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ovwproject\OVWMigration\docs\OVW Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="34"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="37" activeTab="47"/>
   </bookViews>
   <sheets>
     <sheet name="en_au" sheetId="1" r:id="rId1"/>
@@ -769,13 +769,13 @@
     <t>solution-listing-var2</t>
   </si>
   <si>
-    <t>solution-listing-var6</t>
-  </si>
-  <si>
     <t>solution-listing-var8</t>
   </si>
   <si>
     <t>solution-listing-var11</t>
+  </si>
+  <si>
+    <t>solution-listing-var12</t>
   </si>
 </sst>
 </file>
@@ -1139,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1172,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -1200,7 +1200,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -1214,7 +1214,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -1238,7 +1238,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +1270,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -1298,7 +1298,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -1312,7 +1312,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -1335,7 +1335,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,7 +1367,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -1395,7 +1395,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -1409,7 +1409,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -1432,7 +1432,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,7 +1464,7 @@
         <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" t="s">
         <v>84</v>
@@ -1478,7 +1478,7 @@
         <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" t="s">
         <v>84</v>
@@ -1499,7 +1499,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,7 +1531,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -1559,7 +1559,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -1573,7 +1573,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -1596,7 +1596,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,7 +1628,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -1656,7 +1656,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -1670,7 +1670,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -1725,7 +1725,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -1753,7 +1753,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -1767,7 +1767,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -1822,7 +1822,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -1850,7 +1850,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -1864,7 +1864,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -1919,7 +1919,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -1947,7 +1947,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -1961,7 +1961,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -1984,7 +1984,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2016,7 +2016,7 @@
         <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" t="s">
         <v>84</v>
@@ -2030,7 +2030,7 @@
         <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" t="s">
         <v>84</v>
@@ -2051,7 +2051,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2083,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -2111,7 +2111,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -2125,7 +2125,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -2148,7 +2148,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,7 +2180,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -2208,7 +2208,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -2222,7 +2222,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -2277,7 +2277,7 @@
         <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" t="s">
         <v>84</v>
@@ -2291,7 +2291,7 @@
         <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" t="s">
         <v>84</v>
@@ -2312,7 +2312,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,7 +2344,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -2372,7 +2372,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -2386,7 +2386,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -2409,7 +2409,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2441,7 +2441,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -2469,7 +2469,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -2483,7 +2483,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -2506,7 +2506,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,7 +2538,7 @@
         <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" t="s">
         <v>84</v>
@@ -2552,7 +2552,7 @@
         <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" t="s">
         <v>84</v>
@@ -2573,7 +2573,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2605,7 +2605,7 @@
         <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" t="s">
         <v>84</v>
@@ -2619,7 +2619,7 @@
         <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" t="s">
         <v>84</v>
@@ -2640,7 +2640,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2672,7 +2672,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -2700,7 +2700,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -2714,7 +2714,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -2737,7 +2737,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,7 +2769,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -2797,7 +2797,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -2811,7 +2811,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -2834,7 +2834,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2866,7 +2866,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -2894,7 +2894,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -2908,7 +2908,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -2931,7 +2931,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2963,7 +2963,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -2991,7 +2991,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -3005,7 +3005,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -3028,7 +3028,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3060,7 +3060,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -3088,7 +3088,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -3102,7 +3102,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -3125,7 +3125,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3157,7 +3157,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -3185,7 +3185,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -3199,7 +3199,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -3222,7 +3222,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3254,7 +3254,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -3282,7 +3282,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -3296,7 +3296,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -3319,7 +3319,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3351,7 +3351,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -3379,7 +3379,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -3393,7 +3393,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -3416,7 +3416,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3448,7 +3448,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -3476,7 +3476,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -3490,7 +3490,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -3513,7 +3513,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3545,7 +3545,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -3573,7 +3573,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -3587,7 +3587,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -3610,7 +3610,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3642,7 +3642,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -3670,7 +3670,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -3684,7 +3684,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -3707,7 +3707,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3739,7 +3739,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -3767,7 +3767,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -3781,7 +3781,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -3836,7 +3836,7 @@
         <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" t="s">
         <v>84</v>
@@ -3850,7 +3850,7 @@
         <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" t="s">
         <v>84</v>
@@ -3871,7 +3871,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3903,7 +3903,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -3931,7 +3931,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -3945,7 +3945,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -3968,7 +3968,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4000,7 +4000,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -4028,7 +4028,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -4042,7 +4042,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -4065,7 +4065,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4097,7 +4097,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -4125,7 +4125,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -4139,7 +4139,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -4162,7 +4162,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4194,7 +4194,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -4222,7 +4222,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -4236,7 +4236,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -4259,7 +4259,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4291,7 +4291,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -4319,7 +4319,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -4333,7 +4333,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -4356,7 +4356,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4388,7 +4388,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -4416,7 +4416,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -4430,7 +4430,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -4453,7 +4453,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4485,7 +4485,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -4513,7 +4513,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -4527,7 +4527,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -4550,7 +4550,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4582,7 +4582,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -4610,7 +4610,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -4624,7 +4624,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -4647,7 +4647,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4679,7 +4679,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -4707,7 +4707,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -4721,7 +4721,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -4744,7 +4744,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4776,7 +4776,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -4804,7 +4804,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -4818,7 +4818,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -4841,7 +4841,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4873,7 +4873,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -4901,7 +4901,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -4915,7 +4915,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -4938,7 +4938,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4970,7 +4970,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -4998,7 +4998,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -5012,7 +5012,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -5034,7 +5034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -5067,7 +5067,7 @@
         <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" t="s">
         <v>84</v>
@@ -5081,7 +5081,7 @@
         <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" t="s">
         <v>84</v>
@@ -5102,7 +5102,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5134,7 +5134,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -5162,7 +5162,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -5176,7 +5176,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -5199,7 +5199,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5231,7 +5231,7 @@
         <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" t="s">
         <v>84</v>
@@ -5245,7 +5245,7 @@
         <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" t="s">
         <v>84</v>
@@ -5266,7 +5266,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5298,7 +5298,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -5326,7 +5326,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -5340,7 +5340,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -5363,7 +5363,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5395,7 +5395,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -5423,7 +5423,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -5437,7 +5437,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -5460,7 +5460,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5492,7 +5492,7 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -5520,7 +5520,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -5534,7 +5534,7 @@
         <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>

</xml_diff>